<commit_message>
Updated filtering functionality and excluded admin from all_sales
</commit_message>
<xml_diff>
--- a/sales.xlsx
+++ b/sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oussa\Desktop\crm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B8BD6-B08C-459F-B8FD-06E0B599E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3338BB8-8C7C-4006-A480-7527B12B1683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{7C015D74-3DF2-45E7-8CCA-F9B984A8FD62}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" xr2:uid="{7C015D74-3DF2-45E7-8CCA-F9B984A8FD62}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -9815,7 +9815,7 @@
   <dimension ref="A1:F3230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3230"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>